<commit_message>
Update for first Test
Update for first Test
</commit_message>
<xml_diff>
--- a/Docs/Conception technique MVC.xlsx
+++ b/Docs/Conception technique MVC.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projets\2017-12-04_projetgroupe_wetransfer\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dleger/Desktop/AFORMAC03-DLEGER/SITES &amp; EXERCICES/Projets/Groupe/Projet_wetransfer/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29620" yWindow="760" windowWidth="28800" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,15 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$H$10</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,9 +77,6 @@
     <t>deveandcie.fr</t>
   </si>
   <si>
-    <t>HomeController</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -132,11 +135,14 @@
 $_POST['dest_message']
 $_POST['file_name']</t>
   </si>
+  <si>
+    <t>HomePageController</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,7 +216,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -219,136 +225,136 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -744,27 +750,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="31" style="2" customWidth="1"/>
-    <col min="8" max="8" width="53.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="53.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -780,7 +786,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -794,7 +800,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -805,7 +811,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
@@ -832,7 +838,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" s="23"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -843,7 +849,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>13</v>
       </c>
@@ -858,7 +864,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>12</v>
@@ -869,35 +875,35 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="90" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="96" x14ac:dyDescent="0.15">
       <c r="A7" s="18"/>
       <c r="B7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
@@ -905,25 +911,25 @@
         <v>9</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="48" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
@@ -931,29 +937,29 @@
         <v>9</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
@@ -961,25 +967,25 @@
         <v>9</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -993,7 +999,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1008,7 +1014,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1023,7 +1029,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1032,7 +1038,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>

</xml_diff>